<commit_message>
Updated experiment schedule for spring 2020.
</commit_message>
<xml_diff>
--- a/Experiment Schedule.xlsx
+++ b/Experiment Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mskblackbelt/Library/Mobile Documents/com~apple~CloudDocs/iCloud Drive/Teaching/CHEM357/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D15237-D9FA-004D-85B0-1652772ACEE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A4B053-BEF9-614A-8872-1C59E7B57C97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="17100" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
   <si>
     <t>GROUP 1</t>
   </si>
@@ -76,16 +76,13 @@
   </si>
   <si>
     <t>CompChem intro</t>
-  </si>
-  <si>
-    <t>HCL/DCL comp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,7 +144,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -164,37 +161,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color theme="4"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color theme="4"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color theme="4"/>
-      </right>
-      <top style="thick">
-        <color theme="4"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -202,18 +168,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent2" xfId="2" builtinId="35"/>
@@ -534,10 +496,10 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="3" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -546,285 +508,285 @@
     <col min="6" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" thickBot="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>43857</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43859</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <f>B2+7</f>
+        <v>43864</v>
+      </c>
+      <c r="C3" s="2">
+        <f>C2+7</f>
+        <v>43866</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <f>B3+7</f>
+        <v>43871</v>
+      </c>
+      <c r="C4" s="2">
+        <f>C3+7+7</f>
+        <v>43880</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <f>B4+7+7</f>
+        <v>43885</v>
+      </c>
+      <c r="C5" s="2">
+        <f>C4+7</f>
+        <v>43887</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <f>B5+7</f>
+        <v>43892</v>
+      </c>
+      <c r="C6" s="2">
+        <f>C5+7</f>
+        <v>43894</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <f>B6+7</f>
+        <v>43899</v>
+      </c>
+      <c r="C7" s="2">
+        <f>C6+7</f>
+        <v>43901</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" ref="B8:C13" si="0">B7+7</f>
+        <v>43906</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>43908</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" si="0"/>
+        <v>43913</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>43915</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
+        <v>43920</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>43922</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
+        <v>43927</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>43929</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="21" thickTop="1">
-      <c r="A2" s="10">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
+        <v>43934</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>43936</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2">
-        <v>43857</v>
-      </c>
-      <c r="E2" s="2">
-        <v>43859</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="20">
-      <c r="A3" s="9">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>43941</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>43943</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2">
-        <f>D2+7</f>
-        <v>43864</v>
-      </c>
-      <c r="E3" s="2">
-        <f>E2+7</f>
-        <v>43866</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="20">
-      <c r="A4" s="9">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2">
-        <f>D3+7</f>
-        <v>43871</v>
-      </c>
-      <c r="E4" s="2">
-        <f>E3+7+7</f>
-        <v>43880</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="20">
-      <c r="A5" s="9">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2">
-        <f>D4+7+7</f>
-        <v>43885</v>
-      </c>
-      <c r="E5" s="2">
-        <f>E4+7</f>
-        <v>43887</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="20">
-      <c r="A6" s="9">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2">
-        <f>D5+7</f>
-        <v>43892</v>
-      </c>
-      <c r="E6" s="2">
-        <f>E5+7</f>
-        <v>43894</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="20">
-      <c r="A7" s="9">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2">
-        <f>D6+7</f>
-        <v>43899</v>
-      </c>
-      <c r="E7" s="2">
-        <f>E6+7</f>
-        <v>43901</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="20">
-      <c r="A8" s="9">
+      <c r="B14" s="2">
+        <f>B13+7</f>
+        <v>43948</v>
+      </c>
+      <c r="C14" s="2">
+        <f>C13+7</f>
+        <v>43950</v>
+      </c>
+      <c r="D14" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2">
-        <f t="shared" ref="D8:E13" si="0">D7+7</f>
-        <v>43906</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" si="0"/>
-        <v>43908</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="20">
-      <c r="A9" s="9">
+      <c r="B15" s="2">
+        <f>B14+7</f>
+        <v>43955</v>
+      </c>
+      <c r="C15" s="2">
+        <f>C14+7</f>
+        <v>43957</v>
+      </c>
+      <c r="D15" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="2">
-        <f t="shared" si="0"/>
-        <v>43913</v>
-      </c>
-      <c r="E9" s="2">
-        <f t="shared" si="0"/>
-        <v>43915</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="20">
-      <c r="A10" s="9">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="2">
-        <f t="shared" si="0"/>
-        <v>43920</v>
-      </c>
-      <c r="E10" s="2">
-        <f t="shared" si="0"/>
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="20">
-      <c r="A11" s="9">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2">
-        <f t="shared" si="0"/>
-        <v>43927</v>
-      </c>
-      <c r="E11" s="2">
-        <f t="shared" si="0"/>
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="20">
-      <c r="A12" s="9">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2">
-        <f t="shared" si="0"/>
-        <v>43934</v>
-      </c>
-      <c r="E12" s="2">
-        <f t="shared" si="0"/>
-        <v>43936</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="20">
-      <c r="A13" s="9">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="2">
-        <f t="shared" si="0"/>
-        <v>43941</v>
-      </c>
-      <c r="E13" s="2">
-        <f t="shared" si="0"/>
-        <v>43943</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="20">
-      <c r="A14" s="9">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="2">
-        <f>D13+7</f>
-        <v>43948</v>
-      </c>
-      <c r="E14" s="2">
-        <f>E13+7</f>
-        <v>43950</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="20">
-      <c r="A15" s="9">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="E15" t="s">
         <v>8</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="2">
-        <f>D14+7</f>
-        <v>43955</v>
-      </c>
-      <c r="E15" s="2">
-        <f>E14+7</f>
-        <v>43957</v>
       </c>
     </row>
   </sheetData>

</xml_diff>